<commit_message>
pianist and drummer working
</commit_message>
<xml_diff>
--- a/finances/expenses.xlsx
+++ b/finances/expenses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cakan\Documents\GitHub\CompaneroBots\finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6C9F5B-2259-480F-AFDD-A5C8E0581E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67A82F7-8603-4B0C-98E4-13302266E0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
   <si>
     <t>Person</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>2x RGB matrix + 4pin konektor + 2x driver na krokové motory</t>
+  </si>
+  <si>
+    <t>3x ESP32</t>
+  </si>
+  <si>
+    <t>techfun</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -531,7 +537,7 @@
       </c>
       <c r="G2" s="6">
         <f>SUM(C:C)</f>
-        <v>330.99</v>
+        <v>354.84000000000003</v>
       </c>
       <c r="H2" s="6"/>
     </row>
@@ -633,7 +639,7 @@
       </c>
       <c r="H7" s="1">
         <f>SUMIF(A:A,G7,C:C)</f>
-        <v>135.44</v>
+        <v>159.29</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -875,6 +881,20 @@
       <c r="D26" s="3" t="str">
         <f>HYPERLINK("invoices/techfun_202518089.pdf","techfun")</f>
         <v>techfun</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1">
+        <v>23.85</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>